<commit_message>
Neural Network with Regression Implemented
</commit_message>
<xml_diff>
--- a/Networks/Parte1/Excel/Parte1-FeedForward.xlsx
+++ b/Networks/Parte1/Excel/Parte1-FeedForward.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Layer0" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Layer1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -454,10 +453,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.2691743678825218</v>
+        <v>-0.0772216348024467</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.505401542077316</v>
+        <v>-0.4719153656784933</v>
       </c>
     </row>
     <row r="3">
@@ -467,10 +466,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.6167530004561141</v>
+        <v>-0.3244479731105778</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.3539426637885221</v>
+        <v>-0.339491093008931</v>
       </c>
     </row>
     <row r="4">
@@ -480,80 +479,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3604059411213281</v>
+        <v>-0.73218848422015</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1323584180140236</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Neuron0</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Neuron1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Bias</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-0.3860017584442113</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-0.737720955035039</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Weight0</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.97990346528234</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.9008380220540926</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Weight1</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.1658181856286514</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.2733269519144756</v>
+        <v>-0.1255680597707436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Files can be sent to scripts as arguments from de terminal
</commit_message>
<xml_diff>
--- a/Networks/Parte1/Excel/Parte1-FeedForward.xlsx
+++ b/Networks/Parte1/Excel/Parte1-FeedForward.xlsx
@@ -454,10 +454,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.7375907031143634</v>
+        <v>-0.9633038705127712</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.9005962309116796</v>
+        <v>-0.2889435717831422</v>
       </c>
     </row>
     <row r="3">
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.8723468145766988</v>
+        <v>0.8870168358053145</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8042947526201276</v>
+        <v>0.3890749122423709</v>
       </c>
     </row>
     <row r="4">
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.9801824435318121</v>
+        <v>-0.2053854463661027</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3336830083986406</v>
+        <v>-0.3121330545868284</v>
       </c>
     </row>
   </sheetData>
@@ -524,10 +524,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.7044491127281226</v>
+        <v>-0.3778835960970965</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1534517071763384</v>
+        <v>-0.6208671227570343</v>
       </c>
     </row>
     <row r="3">
@@ -537,10 +537,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.08626087767438961</v>
+        <v>-0.7967644956872764</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.05694272229805519</v>
+        <v>0.9125765515905209</v>
       </c>
     </row>
     <row r="4">
@@ -550,10 +550,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.2830037317103378</v>
+        <v>-0.2199469702406884</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1863367416136543</v>
+        <v>-0.3915850869071731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>